<commit_message>
make source for each partition instead each table
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h00292103\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\cs-tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>配置项</t>
   </si>
@@ -175,6 +175,50 @@
   </si>
   <si>
     <t>channel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>need_create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>partition_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -208,7 +252,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -546,35 +590,43 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="42" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -587,26 +639,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>15</v>
+      <c r="B1" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>12</v>
@@ -614,56 +667,71 @@
       <c r="D1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
       <c r="C2" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3">
-        <v>2</v>
-      </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
       <c r="C4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
         <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>